<commit_message>
Arummando um indicador da dashboard
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Requisitos/Pasta1.xlsx
+++ b/Documentação/Planilha de Requisitos/Pasta1.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{E7F64981-A4A7-49AC-91BF-C87BCEF6CEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5E1CC45-E22C-47B3-8615-9D724E91A59C}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E5E1CC45-E22C-47B3-8615-9D724E91A59C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -970,7 +970,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>